<commit_message>
Updated email addresses in users sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepti\Desktop\imperium_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779B7DB6-9994-43C2-971A-9792ABABA231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB965547-ACEA-475F-9B34-C63510D18901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{730DF1DB-C3E8-4555-8E91-E2AF207B1844}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{730DF1DB-C3E8-4555-8E91-E2AF207B1844}"/>
   </bookViews>
   <sheets>
-    <sheet name="scores" sheetId="1" r:id="rId1"/>
-    <sheet name="attendance" sheetId="2" r:id="rId2"/>
+    <sheet name="attendance" sheetId="2" r:id="rId1"/>
+    <sheet name="users" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -46,57 +46,95 @@
     <t>Siddharth</t>
   </si>
   <si>
+    <t>Deepti</t>
+  </si>
+  <si>
+    <t>Komal</t>
+  </si>
+  <si>
+    <t>Bhakti</t>
+  </si>
+  <si>
+    <t>Rimjhim</t>
+  </si>
+  <si>
+    <t>23-062025</t>
+  </si>
+  <si>
+    <t>29-062025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present </t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>bhakti1@gmail.com</t>
-  </si>
-  <si>
-    <t>deepti1@gmail.com</t>
-  </si>
-  <si>
-    <t>rakshita1@gmail.com</t>
-  </si>
-  <si>
-    <t>siddharth1@gmail.com</t>
-  </si>
-  <si>
-    <t>komal1@gmail.com</t>
-  </si>
-  <si>
-    <t>rhimjhim1@gmail.com</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Emoji</t>
   </si>
   <si>
     <t>Score</t>
   </si>
   <si>
-    <t xml:space="preserve">Bhakti </t>
-  </si>
-  <si>
-    <t>Deepti</t>
-  </si>
-  <si>
-    <t>Komal</t>
-  </si>
-  <si>
-    <t>Bhakti</t>
-  </si>
-  <si>
-    <t>Rimjhim</t>
-  </si>
-  <si>
-    <t>23-062025</t>
-  </si>
-  <si>
-    <t>29-062025</t>
+    <t>bhaktishinde@gmail.com</t>
+  </si>
+  <si>
+    <t>Imperium</t>
+  </si>
+  <si>
+    <t>🌸</t>
+  </si>
+  <si>
+    <t>dhanwatedeepti2@gmail.com</t>
+  </si>
+  <si>
+    <t>rakshita@gmail.com</t>
+  </si>
+  <si>
+    <t>👑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siddharth </t>
+  </si>
+  <si>
+    <t>siddharthtayade2602@gmail.com</t>
+  </si>
+  <si>
+    <t>😎</t>
+  </si>
+  <si>
+    <t>rimjhim@gmail.com</t>
+  </si>
+  <si>
+    <t>komal@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,12 +169,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,114 +497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3182E635-589C-4E43-847F-BAC8D7F7369E}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A980DF88-5763-4CA4-A42D-C92900A7A250}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{09337CA0-B620-4337-808F-F2BD03E55488}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{27A919C5-6BCC-46F9-ADCA-D3856F146A88}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{4F9A39DC-2120-4C16-BD63-38AED7D626CC}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{52052291-63E6-42C9-8100-DEE1A9A6B562}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{809153C1-4554-4949-8A04-EA4C32A2B07C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64756EEA-2FCD-41EE-BD1B-2439E6CEC939}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,163 +515,312 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1">
         <v>45839</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>45847</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>45856</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>45861</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F348D943-D9B1-4B08-B893-AC13C711CBFB}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{73B83573-EAEA-48CE-8495-1D57FECC5851}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{5009BA63-2844-4162-A0B1-8FAE21CA165C}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{4CEA35A2-5879-4BB0-939F-4E8A80DF39A8}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{2113626F-DBD8-43D1-B5F0-11BCED1AF087}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{B13EEE1A-1193-4254-9D8E-121973E05BBF}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{FB7D0D57-717E-4802-9C25-9B94CECBC561}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>